<commit_message>
fechas locas y petaca_report
</commit_message>
<xml_diff>
--- a/PyFrame/reports/report_excel/user_report_template.xlsx
+++ b/PyFrame/reports/report_excel/user_report_template.xlsx
@@ -14,18 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>Summary</t>
-  </si>
-  <si>
-    <t>Executed Test Cases</t>
-  </si>
-  <si>
-    <t>Passed Test Cases</t>
-  </si>
-  <si>
-    <t>Failed Test Cases</t>
   </si>
   <si>
     <t>Tester</t>
@@ -137,12 +128,6 @@
     </r>
   </si>
   <si>
-    <t>Number of Test Cases</t>
-  </si>
-  <si>
-    <t>Test Execution Status</t>
-  </si>
-  <si>
     <t>&lt;Number of Passed|Failed|Blocked TCs&gt;/
 &lt;Total Test Cases&gt;*100
 e.g: 100%</t>
@@ -170,9 +155,6 @@
     <t>&lt;Component_Name_1&gt;</t>
   </si>
   <si>
-    <t>Skipped Test Cases</t>
-  </si>
-  <si>
     <t>Test Cases</t>
   </si>
   <si>
@@ -182,9 +164,6 @@
     <t>Scenario</t>
   </si>
   <si>
-    <t>Automatic / Manual</t>
-  </si>
-  <si>
     <t>Duration</t>
   </si>
   <si>
@@ -207,13 +186,31 @@
   </si>
   <si>
     <t>&lt;Test case steps&gt;</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>Skipped</t>
+  </si>
+  <si>
+    <t>Executed</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Execution %</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -251,8 +248,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -265,8 +270,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14996795556505021"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -433,11 +444,109 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -454,11 +563,43 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -770,210 +911,211 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.7109375" customWidth="1"/>
-    <col min="8" max="8" width="22" customWidth="1"/>
-    <col min="9" max="9" width="20.5703125" customWidth="1"/>
+    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="40.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="10"/>
+      <c r="A1" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="22"/>
     </row>
     <row r="2" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="14"/>
+      <c r="A2" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="26"/>
     </row>
     <row r="3" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="14"/>
+      <c r="A3" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="26"/>
     </row>
     <row r="4" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="14"/>
+      <c r="A4" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="26"/>
     </row>
     <row r="5" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="14"/>
+      <c r="A5" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="26"/>
     </row>
     <row r="6" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="12"/>
+      <c r="A6" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="24"/>
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="10"/>
-    </row>
-    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="22"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+      <c r="B11" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
     </row>
     <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="10"/>
+      <c r="A14" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="18"/>
+      <c r="E15" s="19"/>
       <c r="F15" s="2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="107.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I16" s="6" t="s">
-        <v>15</v>
+        <v>25</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="15"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C15:E15"/>
     <mergeCell ref="A9:I9"/>
-    <mergeCell ref="A14:I14"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>

</xml_diff>